<commit_message>
Accessing for primary joint angles from simplified model
</commit_message>
<xml_diff>
--- a/specialized-resources/Normative Ranges for Open SIM.xlsx
+++ b/specialized-resources/Normative Ranges for Open SIM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://specialized-my.sharepoint.com/personal/jwilliams_specialized_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\GitHub\spec-opensim\specialized-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{60AF4F97-3803-4E06-A1CB-32C7B9DD7AF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{2362BC6F-2E24-41A8-85E5-0870308205B5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F742B363-7EA9-4F48-B6A7-9CB2CA3B9E7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C9881907-F7FC-48BD-A618-5FD0580897EE}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{C9881907-F7FC-48BD-A618-5FD0580897EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Road" sheetId="1" r:id="rId1"/>
@@ -371,12 +371,36 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -391,14 +415,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFCCCC"/>
+      <color rgb="FFCCFFCC"/>
+      <color rgb="FFCCECFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -709,11 +744,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767523B2-6299-4EE2-978C-0712E652FB6B}">
   <dimension ref="A1:BP10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -741,46 +779,46 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>16</v>
       </c>
       <c r="P1" t="s">
@@ -1150,210 +1188,210 @@
         <v>101.65722514035069</v>
       </c>
     </row>
-    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>7.398354054221949</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="4">
         <v>6.0975630182034486</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="4">
         <v>6.6328829369870235</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="4">
         <v>8.12752918907211</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="4">
         <v>6.9844499616553097</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <v>6.0722376835107088</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="4">
         <v>7.4387232395141503</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <v>3.6596156008620992</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="4">
         <v>5.4095832887317847</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="4">
         <f>J4</f>
         <v>5.4095832887317847</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="4">
         <v>4.6145145759223443</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="4">
         <v>5.6114521550331826</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="4">
         <v>5.9834067235406394</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="4">
         <v>3.8068908232760328</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="4">
         <v>6.1145658755743852</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="4">
         <v>6.3110069870139833</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="4">
         <v>5.5197591234926806</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="4">
         <v>13.604560967985925</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="4">
         <v>10.741766401644689</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="4">
         <v>24.559695852936585</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="4">
         <v>24.175909605215914</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="4">
         <v>16.505342437908805</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="4">
         <v>11.605481861250624</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="4">
         <v>35.868360453930613</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="4">
         <v>5.4764399153655416</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="4">
         <v>2.9617323880912223</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="4">
         <v>2.9014563666430835</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="4">
         <v>2.9762712199168266</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="4">
         <v>3.31780087505931</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="4">
         <v>12.138465885001713</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="4">
         <v>11.471802120009597</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="4">
         <v>5.2046861974534595</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="4">
         <v>29.522718593694623</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="4">
         <v>207.63644533896181</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="4">
         <v>44.206339768893955</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="4">
         <v>34.870599841852524</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="4">
         <v>18.91389781719775</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="4">
         <v>50.078246250835917</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="4">
         <v>53.57584853500915</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="4">
         <v>53.462192251694226</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="4">
         <v>46.425149138966418</v>
       </c>
-      <c r="AQ4">
+      <c r="AQ4" s="4">
         <v>12.060879502540331</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="4">
         <v>3.0986143734232259E-2</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="4">
         <v>5.0487635713864665E-2</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="4">
         <v>4.3271980739607335E-2</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="4">
         <v>3.057439716626759E-2</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="4">
         <v>6.2549797692087281E-2</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="4">
         <v>5.9210646917290902E-2</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="4">
         <v>3.2923527343514808E-2</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="4">
         <v>7.4186007909545923E-2</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="4">
         <v>4.7223253623736944E-2</v>
       </c>
-      <c r="BA4">
+      <c r="BA4" s="4">
         <v>2.084717014083956E-2</v>
       </c>
-      <c r="BB4">
+      <c r="BB4" s="4">
         <v>5.3673390325966713E-2</v>
       </c>
-      <c r="BC4">
+      <c r="BC4" s="4">
         <v>2.6038953060239553E-2</v>
       </c>
-      <c r="BD4">
+      <c r="BD4" s="4">
         <v>2.1172067613975942E-2</v>
       </c>
-      <c r="BE4">
+      <c r="BE4" s="4">
         <v>3.6611323102193297E-2</v>
       </c>
-      <c r="BF4">
+      <c r="BF4" s="4">
         <v>2.1604264439318992E-2</v>
       </c>
-      <c r="BG4">
+      <c r="BG4" s="4">
         <v>0.1893955909097928</v>
       </c>
-      <c r="BH4">
+      <c r="BH4" s="4">
         <v>2.78475793685692E-2</v>
       </c>
-      <c r="BI4">
+      <c r="BI4" s="4">
         <v>1.6879552221785742E-2</v>
       </c>
-      <c r="BJ4">
+      <c r="BJ4" s="4">
         <v>1.5901051413779021E-2</v>
       </c>
-      <c r="BK4">
+      <c r="BK4" s="4">
         <v>1.4791700180311253E-2</v>
       </c>
-      <c r="BL4">
+      <c r="BL4" s="4">
         <v>5.0762615820817373E-3</v>
       </c>
-      <c r="BM4">
+      <c r="BM4" s="4">
         <v>1.4930346645554019E-2</v>
       </c>
-      <c r="BN4">
+      <c r="BN4" s="4">
         <v>6.8277963643856082E-3</v>
       </c>
-      <c r="BO4">
+      <c r="BO4" s="4">
         <v>9.9313577467809466</v>
       </c>
-      <c r="BP4">
+      <c r="BP4" s="4">
         <v>27.397485094722228</v>
       </c>
     </row>
@@ -1920,11 +1958,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F8624A-3110-4856-8D85-CA9B733FB2F1}">
   <dimension ref="A1:BV10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="BG1" workbookViewId="0">
+      <selection activeCell="BV1" sqref="BV1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -1934,7 +1972,7 @@
     <col min="6" max="6" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Further adjusting of matlab scripts for reading data
</commit_message>
<xml_diff>
--- a/specialized-resources/Normative Ranges for Open SIM.xlsx
+++ b/specialized-resources/Normative Ranges for Open SIM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\GitHub\spec-opensim\specialized-resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F742B363-7EA9-4F48-B6A7-9CB2CA3B9E7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC4932F-5636-4876-B04F-BCBBBC94A0F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" xr2:uid="{C9881907-F7FC-48BD-A618-5FD0580897EE}"/>
   </bookViews>
@@ -742,13 +742,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767523B2-6299-4EE2-978C-0712E652FB6B}">
-  <dimension ref="A1:BP10"/>
+  <dimension ref="A1:BP8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -981,971 +981,971 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="2" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B2">
         <v>75.58305826429077</v>
       </c>
-      <c r="C3">
+      <c r="C2">
         <v>96.013453424120129</v>
       </c>
-      <c r="D3">
+      <c r="D2">
         <v>20.496851755851999</v>
       </c>
-      <c r="E3">
+      <c r="E2">
         <v>80.282938143519601</v>
       </c>
-      <c r="F3">
+      <c r="F2">
         <v>78.353169969890075</v>
       </c>
-      <c r="G3">
+      <c r="G2">
         <v>94.826585621688324</v>
       </c>
-      <c r="H3">
+      <c r="H2">
         <v>88.446139193047799</v>
       </c>
-      <c r="I3">
+      <c r="I2">
         <v>69.499996278194374</v>
       </c>
-      <c r="J3">
+      <c r="J2">
         <v>142.45824843504022</v>
       </c>
-      <c r="K3">
-        <f>180-J3</f>
+      <c r="K2">
+        <f>180-J2</f>
         <v>37.541751564959782</v>
       </c>
-      <c r="L3">
+      <c r="L2">
         <v>73.087848738106686</v>
       </c>
-      <c r="M3">
+      <c r="M2">
         <v>63.635102898796717</v>
       </c>
-      <c r="N3">
+      <c r="N2">
         <v>109.14067416107147</v>
       </c>
-      <c r="O3">
+      <c r="O2">
         <v>45.611790245380575</v>
       </c>
-      <c r="P3">
+      <c r="P2">
         <v>45.113013856628392</v>
       </c>
-      <c r="Q3">
+      <c r="Q2">
         <v>82.002906160662832</v>
       </c>
-      <c r="R3">
+      <c r="R2">
         <v>70.49498551622716</v>
       </c>
-      <c r="S3">
+      <c r="S2">
         <v>149.98449146655344</v>
       </c>
-      <c r="T3">
+      <c r="T2">
         <v>-37.128438459330987</v>
       </c>
-      <c r="U3">
+      <c r="U2">
         <v>-2.5908517733673935</v>
       </c>
-      <c r="V3">
+      <c r="V2">
         <v>-19.946058954567512</v>
       </c>
-      <c r="W3">
+      <c r="W2">
         <v>-20.207512921249833</v>
       </c>
-      <c r="X3">
+      <c r="X2">
         <v>-2.9401125490463738</v>
       </c>
-      <c r="Y3">
+      <c r="Y2">
         <v>19.138265502827885</v>
       </c>
-      <c r="Z3">
+      <c r="Z2">
         <v>-23.113794396800721</v>
       </c>
-      <c r="AA3">
+      <c r="AA2">
         <v>-10.695934323875491</v>
       </c>
-      <c r="AB3">
+      <c r="AB2">
         <v>-9.6652869383404187</v>
       </c>
-      <c r="AC3">
+      <c r="AC2">
         <v>-8.6109465371265657</v>
       </c>
-      <c r="AD3">
+      <c r="AD2">
         <v>1.9589355038988443</v>
       </c>
-      <c r="AE3">
+      <c r="AE2">
         <v>24.766310674264538</v>
       </c>
-      <c r="AF3">
+      <c r="AF2">
         <v>48.497502765950713</v>
       </c>
-      <c r="AG3">
+      <c r="AG2">
         <v>12.478595658680758</v>
       </c>
-      <c r="AH3">
+      <c r="AH2">
         <v>426.14688301905682</v>
       </c>
-      <c r="AI3">
+      <c r="AI2">
         <v>418.02684571321242</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ2">
         <v>511.73091354777625</v>
       </c>
-      <c r="AK3">
+      <c r="AK2">
         <v>332.7102616025827</v>
       </c>
-      <c r="AL3">
+      <c r="AL2">
         <v>257.24689191432481</v>
       </c>
-      <c r="AM3">
+      <c r="AM2">
         <v>-89.214782631140295</v>
       </c>
-      <c r="AN3">
+      <c r="AN2">
         <v>697.21020311270081</v>
       </c>
-      <c r="AO3">
+      <c r="AO2">
         <v>64.644739048521103</v>
       </c>
-      <c r="AP3">
+      <c r="AP2">
         <v>497.63315745751044</v>
       </c>
-      <c r="AQ3">
+      <c r="AQ2">
         <v>0.83356710501038644</v>
       </c>
-      <c r="AR3">
+      <c r="AR2">
         <v>0.19341040580788593</v>
       </c>
-      <c r="AS3">
+      <c r="AS2">
         <v>0.66500204436463584</v>
       </c>
-      <c r="AT3">
+      <c r="AT2">
         <v>0.30827577477995438</v>
       </c>
-      <c r="AU3">
+      <c r="AU2">
         <v>0.21120401619860227</v>
       </c>
-      <c r="AV3">
+      <c r="AV2">
         <v>0.81852605116220101</v>
       </c>
-      <c r="AW3">
+      <c r="AW2">
         <v>0.16958744988800564</v>
       </c>
-      <c r="AX3">
+      <c r="AX2">
         <v>0.17396688076925185</v>
       </c>
-      <c r="AY3">
+      <c r="AY2">
         <v>1.1131003577844312</v>
       </c>
-      <c r="AZ3">
+      <c r="AZ2">
         <v>-0.18865770779551555</v>
       </c>
-      <c r="BA3">
+      <c r="BA2">
         <v>0.16174725433167694</v>
       </c>
-      <c r="BB3">
+      <c r="BB2">
         <v>0.75431301493390968</v>
       </c>
-      <c r="BC3">
+      <c r="BC2">
         <v>0.11522714371225014</v>
       </c>
-      <c r="BD3">
+      <c r="BD2">
         <v>0.13894588604407476</v>
       </c>
-      <c r="BE3">
+      <c r="BE2">
         <v>0.47978353708342292</v>
       </c>
-      <c r="BF3">
+      <c r="BF2">
         <v>-6.8761957950092004E-2</v>
       </c>
-      <c r="BG3">
+      <c r="BG2">
         <v>0.12598459143965468</v>
       </c>
-      <c r="BH3">
+      <c r="BH2">
         <v>0.13182063640659264</v>
       </c>
-      <c r="BI3">
+      <c r="BI2">
         <v>-0.12257349145305761</v>
       </c>
-      <c r="BJ3">
+      <c r="BJ2">
         <v>0.13520376147041274</v>
       </c>
-      <c r="BK3">
+      <c r="BK2">
         <v>7.7245590908113171E-2</v>
       </c>
-      <c r="BL3">
+      <c r="BL2">
         <v>6.1188720795088503E-5</v>
       </c>
-      <c r="BM3">
+      <c r="BM2">
         <v>0.15902390109625014</v>
       </c>
-      <c r="BN3">
+      <c r="BN2">
         <v>2.3345628410443343E-2</v>
       </c>
-      <c r="BO3">
+      <c r="BO2">
         <v>87.214029917249476</v>
       </c>
-      <c r="BP3">
+      <c r="BP2">
         <v>101.65722514035069</v>
       </c>
     </row>
-    <row r="4" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="3" spans="1:68" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B3" s="4">
         <v>7.398354054221949</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C3" s="4">
         <v>6.0975630182034486</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D3" s="4">
         <v>6.6328829369870235</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E3" s="4">
         <v>8.12752918907211</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F3" s="4">
         <v>6.9844499616553097</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G3" s="4">
         <v>6.0722376835107088</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H3" s="4">
         <v>7.4387232395141503</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I3" s="4">
         <v>3.6596156008620992</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J3" s="4">
         <v>5.4095832887317847</v>
       </c>
-      <c r="K4" s="4">
-        <f>J4</f>
+      <c r="K3" s="4">
+        <f>J3</f>
         <v>5.4095832887317847</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L3" s="4">
         <v>4.6145145759223443</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M3" s="4">
         <v>5.6114521550331826</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N3" s="4">
         <v>5.9834067235406394</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O3" s="4">
         <v>3.8068908232760328</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P3" s="4">
         <v>6.1145658755743852</v>
       </c>
-      <c r="Q4" s="4">
+      <c r="Q3" s="4">
         <v>6.3110069870139833</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R3" s="4">
         <v>5.5197591234926806</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S3" s="4">
         <v>13.604560967985925</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T3" s="4">
         <v>10.741766401644689</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U3" s="4">
         <v>24.559695852936585</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V3" s="4">
         <v>24.175909605215914</v>
       </c>
-      <c r="W4" s="4">
+      <c r="W3" s="4">
         <v>16.505342437908805</v>
       </c>
-      <c r="X4" s="4">
+      <c r="X3" s="4">
         <v>11.605481861250624</v>
       </c>
-      <c r="Y4" s="4">
+      <c r="Y3" s="4">
         <v>35.868360453930613</v>
       </c>
-      <c r="Z4" s="4">
+      <c r="Z3" s="4">
         <v>5.4764399153655416</v>
       </c>
-      <c r="AA4" s="4">
+      <c r="AA3" s="4">
         <v>2.9617323880912223</v>
       </c>
-      <c r="AB4" s="4">
+      <c r="AB3" s="4">
         <v>2.9014563666430835</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC3" s="4">
         <v>2.9762712199168266</v>
       </c>
-      <c r="AD4" s="4">
+      <c r="AD3" s="4">
         <v>3.31780087505931</v>
       </c>
-      <c r="AE4" s="4">
+      <c r="AE3" s="4">
         <v>12.138465885001713</v>
       </c>
-      <c r="AF4" s="4">
+      <c r="AF3" s="4">
         <v>11.471802120009597</v>
       </c>
-      <c r="AG4" s="4">
+      <c r="AG3" s="4">
         <v>5.2046861974534595</v>
       </c>
-      <c r="AH4" s="4">
+      <c r="AH3" s="4">
         <v>29.522718593694623</v>
       </c>
-      <c r="AI4" s="4">
+      <c r="AI3" s="4">
         <v>207.63644533896181</v>
       </c>
-      <c r="AJ4" s="4">
+      <c r="AJ3" s="4">
         <v>44.206339768893955</v>
       </c>
-      <c r="AK4" s="4">
+      <c r="AK3" s="4">
         <v>34.870599841852524</v>
       </c>
-      <c r="AL4" s="4">
+      <c r="AL3" s="4">
         <v>18.91389781719775</v>
       </c>
-      <c r="AM4" s="4">
+      <c r="AM3" s="4">
         <v>50.078246250835917</v>
       </c>
-      <c r="AN4" s="4">
+      <c r="AN3" s="4">
         <v>53.57584853500915</v>
       </c>
-      <c r="AO4" s="4">
+      <c r="AO3" s="4">
         <v>53.462192251694226</v>
       </c>
-      <c r="AP4" s="4">
+      <c r="AP3" s="4">
         <v>46.425149138966418</v>
       </c>
-      <c r="AQ4" s="4">
+      <c r="AQ3" s="4">
         <v>12.060879502540331</v>
       </c>
-      <c r="AR4" s="4">
+      <c r="AR3" s="4">
         <v>3.0986143734232259E-2</v>
       </c>
-      <c r="AS4" s="4">
+      <c r="AS3" s="4">
         <v>5.0487635713864665E-2</v>
       </c>
-      <c r="AT4" s="4">
+      <c r="AT3" s="4">
         <v>4.3271980739607335E-2</v>
       </c>
-      <c r="AU4" s="4">
+      <c r="AU3" s="4">
         <v>3.057439716626759E-2</v>
       </c>
-      <c r="AV4" s="4">
+      <c r="AV3" s="4">
         <v>6.2549797692087281E-2</v>
       </c>
-      <c r="AW4" s="4">
+      <c r="AW3" s="4">
         <v>5.9210646917290902E-2</v>
       </c>
-      <c r="AX4" s="4">
+      <c r="AX3" s="4">
         <v>3.2923527343514808E-2</v>
       </c>
-      <c r="AY4" s="4">
+      <c r="AY3" s="4">
         <v>7.4186007909545923E-2</v>
       </c>
-      <c r="AZ4" s="4">
+      <c r="AZ3" s="4">
         <v>4.7223253623736944E-2</v>
       </c>
-      <c r="BA4" s="4">
+      <c r="BA3" s="4">
         <v>2.084717014083956E-2</v>
       </c>
-      <c r="BB4" s="4">
+      <c r="BB3" s="4">
         <v>5.3673390325966713E-2</v>
       </c>
-      <c r="BC4" s="4">
+      <c r="BC3" s="4">
         <v>2.6038953060239553E-2</v>
       </c>
-      <c r="BD4" s="4">
+      <c r="BD3" s="4">
         <v>2.1172067613975942E-2</v>
       </c>
-      <c r="BE4" s="4">
+      <c r="BE3" s="4">
         <v>3.6611323102193297E-2</v>
       </c>
-      <c r="BF4" s="4">
+      <c r="BF3" s="4">
         <v>2.1604264439318992E-2</v>
       </c>
-      <c r="BG4" s="4">
+      <c r="BG3" s="4">
         <v>0.1893955909097928</v>
       </c>
-      <c r="BH4" s="4">
+      <c r="BH3" s="4">
         <v>2.78475793685692E-2</v>
       </c>
-      <c r="BI4" s="4">
+      <c r="BI3" s="4">
         <v>1.6879552221785742E-2</v>
       </c>
-      <c r="BJ4" s="4">
+      <c r="BJ3" s="4">
         <v>1.5901051413779021E-2</v>
       </c>
-      <c r="BK4" s="4">
+      <c r="BK3" s="4">
         <v>1.4791700180311253E-2</v>
       </c>
-      <c r="BL4" s="4">
+      <c r="BL3" s="4">
         <v>5.0762615820817373E-3</v>
       </c>
-      <c r="BM4" s="4">
+      <c r="BM3" s="4">
         <v>1.4930346645554019E-2</v>
       </c>
-      <c r="BN4" s="4">
+      <c r="BN3" s="4">
         <v>6.8277963643856082E-3</v>
       </c>
-      <c r="BO4" s="4">
+      <c r="BO3" s="4">
         <v>9.9313577467809466</v>
       </c>
-      <c r="BP4" s="4">
+      <c r="BP3" s="4">
         <v>27.397485094722228</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="4" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
-        <f>B3+B4</f>
+      <c r="B4">
+        <f>B2+B3</f>
         <v>82.981412318512724</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:BO6" si="0">C3+C4</f>
+      <c r="C4">
+        <f t="shared" ref="C4:BO4" si="0">C2+C3</f>
         <v>102.11101644232357</v>
       </c>
-      <c r="D6">
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>27.129734692839023</v>
       </c>
-      <c r="E6">
+      <c r="E4">
         <f t="shared" si="0"/>
         <v>88.410467332591708</v>
       </c>
-      <c r="F6">
+      <c r="F4">
         <f t="shared" si="0"/>
         <v>85.33761993154539</v>
       </c>
-      <c r="G6">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>100.89882330519903</v>
       </c>
-      <c r="H6">
+      <c r="H4">
         <f t="shared" si="0"/>
         <v>95.884862432561945</v>
       </c>
-      <c r="I6">
+      <c r="I4">
         <f t="shared" si="0"/>
         <v>73.15961187905647</v>
       </c>
-      <c r="J6">
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>147.86783172377201</v>
       </c>
-      <c r="K6">
-        <f>180-J6</f>
+      <c r="K4">
+        <f>180-J4</f>
         <v>32.132168276227986</v>
       </c>
-      <c r="L6">
+      <c r="L4">
         <f t="shared" si="0"/>
         <v>77.702363314029029</v>
       </c>
-      <c r="M6">
+      <c r="M4">
         <f t="shared" si="0"/>
         <v>69.246555053829894</v>
       </c>
-      <c r="N6">
+      <c r="N4">
         <f t="shared" si="0"/>
         <v>115.12408088461211</v>
       </c>
-      <c r="O6">
+      <c r="O4">
         <f t="shared" si="0"/>
         <v>49.41868106865661</v>
       </c>
-      <c r="P6">
+      <c r="P4">
         <f t="shared" si="0"/>
         <v>51.227579732202777</v>
       </c>
-      <c r="Q6">
+      <c r="Q4">
         <f t="shared" si="0"/>
         <v>88.313913147676814</v>
       </c>
-      <c r="R6">
+      <c r="R4">
         <f t="shared" si="0"/>
         <v>76.014744639719837</v>
       </c>
-      <c r="S6">
+      <c r="S4">
         <f t="shared" si="0"/>
         <v>163.58905243453935</v>
       </c>
-      <c r="T6">
+      <c r="T4">
         <f t="shared" si="0"/>
         <v>-26.386672057686297</v>
       </c>
-      <c r="U6">
+      <c r="U4">
         <f t="shared" si="0"/>
         <v>21.968844079569191</v>
       </c>
-      <c r="V6">
+      <c r="V4">
         <f t="shared" si="0"/>
         <v>4.2298506506484017</v>
       </c>
-      <c r="W6">
+      <c r="W4">
         <f t="shared" si="0"/>
         <v>-3.7021704833410283</v>
       </c>
-      <c r="X6">
+      <c r="X4">
         <f t="shared" si="0"/>
         <v>8.6653693122042501</v>
       </c>
-      <c r="Y6">
+      <c r="Y4">
         <f t="shared" si="0"/>
         <v>55.006625956758498</v>
       </c>
-      <c r="Z6">
+      <c r="Z4">
         <f t="shared" si="0"/>
         <v>-17.637354481435178</v>
       </c>
-      <c r="AA6">
+      <c r="AA4">
         <f t="shared" si="0"/>
         <v>-7.7342019357842684</v>
       </c>
-      <c r="AB6">
+      <c r="AB4">
         <f t="shared" si="0"/>
         <v>-6.7638305716973353</v>
       </c>
-      <c r="AC6">
+      <c r="AC4">
         <f t="shared" si="0"/>
         <v>-5.634675317209739</v>
       </c>
-      <c r="AD6">
+      <c r="AD4">
         <f t="shared" si="0"/>
         <v>5.2767363789581543</v>
       </c>
-      <c r="AE6">
+      <c r="AE4">
         <f t="shared" si="0"/>
         <v>36.904776559266253</v>
       </c>
-      <c r="AF6">
+      <c r="AF4">
         <f t="shared" si="0"/>
         <v>59.969304885960312</v>
       </c>
-      <c r="AG6">
+      <c r="AG4">
         <f t="shared" si="0"/>
         <v>17.683281856134219</v>
       </c>
-      <c r="AH6">
+      <c r="AH4">
         <f t="shared" si="0"/>
         <v>455.66960161275142</v>
       </c>
-      <c r="AI6">
+      <c r="AI4">
         <f t="shared" si="0"/>
         <v>625.66329105217426</v>
       </c>
-      <c r="AJ6">
+      <c r="AJ4">
         <f t="shared" si="0"/>
         <v>555.93725331667019</v>
       </c>
-      <c r="AK6">
+      <c r="AK4">
         <f t="shared" si="0"/>
         <v>367.58086144443524</v>
       </c>
-      <c r="AL6">
+      <c r="AL4">
         <f t="shared" si="0"/>
         <v>276.16078973152253</v>
       </c>
-      <c r="AM6">
+      <c r="AM4">
         <f t="shared" si="0"/>
         <v>-39.136536380304378</v>
       </c>
-      <c r="AN6">
+      <c r="AN4">
         <f t="shared" si="0"/>
         <v>750.78605164771</v>
       </c>
-      <c r="AO6">
+      <c r="AO4">
         <f t="shared" si="0"/>
         <v>118.10693130021534</v>
       </c>
-      <c r="AP6">
+      <c r="AP4">
         <f t="shared" si="0"/>
         <v>544.05830659647688</v>
       </c>
-      <c r="AQ6">
+      <c r="AQ4">
         <f t="shared" si="0"/>
         <v>12.894446607550718</v>
       </c>
-      <c r="AR6">
+      <c r="AR4">
         <f t="shared" si="0"/>
         <v>0.22439654954211818</v>
       </c>
-      <c r="AS6">
+      <c r="AS4">
         <f t="shared" si="0"/>
         <v>0.71548968007850045</v>
       </c>
-      <c r="AT6">
+      <c r="AT4">
         <f t="shared" si="0"/>
         <v>0.35154775551956174</v>
       </c>
-      <c r="AU6">
+      <c r="AU4">
         <f t="shared" si="0"/>
         <v>0.24177841336486985</v>
       </c>
-      <c r="AV6">
+      <c r="AV4">
         <f t="shared" si="0"/>
         <v>0.88107584885428825</v>
       </c>
-      <c r="AW6">
+      <c r="AW4">
         <f t="shared" si="0"/>
         <v>0.22879809680529656</v>
       </c>
-      <c r="AX6">
+      <c r="AX4">
         <f t="shared" si="0"/>
         <v>0.20689040811276665</v>
       </c>
-      <c r="AY6">
+      <c r="AY4">
         <f t="shared" si="0"/>
         <v>1.1872863656939772</v>
       </c>
-      <c r="AZ6">
+      <c r="AZ4">
         <f t="shared" si="0"/>
         <v>-0.14143445417177861</v>
       </c>
-      <c r="BA6">
+      <c r="BA4">
         <f t="shared" si="0"/>
         <v>0.1825944244725165</v>
       </c>
-      <c r="BB6">
+      <c r="BB4">
         <f t="shared" si="0"/>
         <v>0.80798640525987642</v>
       </c>
-      <c r="BC6">
+      <c r="BC4">
         <f t="shared" si="0"/>
         <v>0.14126609677248969</v>
       </c>
-      <c r="BD6">
+      <c r="BD4">
         <f t="shared" si="0"/>
         <v>0.1601179536580507</v>
       </c>
-      <c r="BE6">
+      <c r="BE4">
         <f t="shared" si="0"/>
         <v>0.5163948601856162</v>
       </c>
-      <c r="BF6">
+      <c r="BF4">
         <f t="shared" si="0"/>
         <v>-4.7157693510773008E-2</v>
       </c>
-      <c r="BG6">
+      <c r="BG4">
         <f t="shared" si="0"/>
         <v>0.31538018234944748</v>
       </c>
-      <c r="BH6">
+      <c r="BH4">
         <f t="shared" si="0"/>
         <v>0.15966821577516183</v>
       </c>
-      <c r="BI6">
+      <c r="BI4">
         <f t="shared" si="0"/>
         <v>-0.10569393923127188</v>
       </c>
-      <c r="BJ6">
+      <c r="BJ4">
         <f t="shared" si="0"/>
         <v>0.15110481288419175</v>
       </c>
-      <c r="BK6">
+      <c r="BK4">
         <f t="shared" si="0"/>
         <v>9.2037291088424428E-2</v>
       </c>
-      <c r="BL6">
+      <c r="BL4">
         <f t="shared" si="0"/>
         <v>5.1374503028768261E-3</v>
       </c>
-      <c r="BM6">
+      <c r="BM4">
         <f t="shared" si="0"/>
         <v>0.17395424774180415</v>
       </c>
-      <c r="BN6">
+      <c r="BN4">
         <f t="shared" si="0"/>
         <v>3.0173424774828952E-2</v>
       </c>
-      <c r="BO6">
+      <c r="BO4">
         <f t="shared" si="0"/>
         <v>97.145387664030423</v>
       </c>
-      <c r="BP6">
-        <f t="shared" ref="BP6" si="1">BP3+BP4</f>
+      <c r="BP4">
+        <f t="shared" ref="BP4" si="1">BP2+BP3</f>
         <v>129.05471023507292</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
-        <f>B3-B4</f>
+      <c r="B5">
+        <f>B2-B3</f>
         <v>68.184704210068816</v>
       </c>
-      <c r="C7">
-        <f t="shared" ref="C7:BO7" si="2">C3-C4</f>
+      <c r="C5">
+        <f t="shared" ref="C5:BO5" si="2">C2-C3</f>
         <v>89.915890405916684</v>
       </c>
-      <c r="D7">
+      <c r="D5">
         <f t="shared" si="2"/>
         <v>13.863968818864976</v>
       </c>
-      <c r="E7">
+      <c r="E5">
         <f t="shared" si="2"/>
         <v>72.155408954447495</v>
       </c>
-      <c r="F7">
+      <c r="F5">
         <f t="shared" si="2"/>
         <v>71.36872000823476</v>
       </c>
-      <c r="G7">
+      <c r="G5">
         <f t="shared" si="2"/>
         <v>88.754347938177617</v>
       </c>
-      <c r="H7">
+      <c r="H5">
         <f t="shared" si="2"/>
         <v>81.007415953533652</v>
       </c>
-      <c r="I7">
+      <c r="I5">
         <f t="shared" si="2"/>
         <v>65.840380677332277</v>
       </c>
-      <c r="J7">
+      <c r="J5">
         <f t="shared" si="2"/>
         <v>137.04866514630842</v>
       </c>
-      <c r="K7">
-        <f>180-J7</f>
+      <c r="K5">
+        <f>180-J5</f>
         <v>42.951334853691577</v>
       </c>
-      <c r="L7">
+      <c r="L5">
         <f t="shared" si="2"/>
         <v>68.473334162184344</v>
       </c>
-      <c r="M7">
+      <c r="M5">
         <f t="shared" si="2"/>
         <v>58.023650743763532</v>
       </c>
-      <c r="N7">
+      <c r="N5">
         <f t="shared" si="2"/>
         <v>103.15726743753083</v>
       </c>
-      <c r="O7">
+      <c r="O5">
         <f t="shared" si="2"/>
         <v>41.80489942210454</v>
       </c>
-      <c r="P7">
+      <c r="P5">
         <f t="shared" si="2"/>
         <v>38.998447981054007</v>
       </c>
-      <c r="Q7">
+      <c r="Q5">
         <f t="shared" si="2"/>
         <v>75.691899173648849</v>
       </c>
-      <c r="R7">
+      <c r="R5">
         <f t="shared" si="2"/>
         <v>64.975226392734484</v>
       </c>
-      <c r="S7">
+      <c r="S5">
         <f t="shared" si="2"/>
         <v>136.37993049856752</v>
       </c>
-      <c r="T7">
+      <c r="T5">
         <f t="shared" si="2"/>
         <v>-47.870204860975676</v>
       </c>
-      <c r="U7">
+      <c r="U5">
         <f t="shared" si="2"/>
         <v>-27.150547626303979</v>
       </c>
-      <c r="V7">
+      <c r="V5">
         <f t="shared" si="2"/>
         <v>-44.121968559783426</v>
       </c>
-      <c r="W7">
+      <c r="W5">
         <f t="shared" si="2"/>
         <v>-36.712855359158638</v>
       </c>
-      <c r="X7">
+      <c r="X5">
         <f t="shared" si="2"/>
         <v>-14.545594410296998</v>
       </c>
-      <c r="Y7">
+      <c r="Y5">
         <f t="shared" si="2"/>
         <v>-16.730094951102728</v>
       </c>
-      <c r="Z7">
+      <c r="Z5">
         <f t="shared" si="2"/>
         <v>-28.590234312166263</v>
       </c>
-      <c r="AA7">
+      <c r="AA5">
         <f t="shared" si="2"/>
         <v>-13.657666711966714</v>
       </c>
-      <c r="AB7">
+      <c r="AB5">
         <f t="shared" si="2"/>
         <v>-12.566743304983502</v>
       </c>
-      <c r="AC7">
+      <c r="AC5">
         <f t="shared" si="2"/>
         <v>-11.587217757043392</v>
       </c>
-      <c r="AD7">
+      <c r="AD5">
         <f t="shared" si="2"/>
         <v>-1.3588653711604657</v>
       </c>
-      <c r="AE7">
+      <c r="AE5">
         <f t="shared" si="2"/>
         <v>12.627844789262825</v>
       </c>
-      <c r="AF7">
+      <c r="AF5">
         <f t="shared" si="2"/>
         <v>37.025700645941114</v>
       </c>
-      <c r="AG7">
+      <c r="AG5">
         <f t="shared" si="2"/>
         <v>7.2739094612272988</v>
       </c>
-      <c r="AH7">
+      <c r="AH5">
         <f t="shared" si="2"/>
         <v>396.62416442536221</v>
       </c>
-      <c r="AI7">
+      <c r="AI5">
         <f t="shared" si="2"/>
         <v>210.39040037425062</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ5">
         <f t="shared" si="2"/>
         <v>467.52457377888231</v>
       </c>
-      <c r="AK7">
+      <c r="AK5">
         <f t="shared" si="2"/>
         <v>297.83966176073017</v>
       </c>
-      <c r="AL7">
+      <c r="AL5">
         <f t="shared" si="2"/>
         <v>238.33299409712706</v>
       </c>
-      <c r="AM7">
+      <c r="AM5">
         <f t="shared" si="2"/>
         <v>-139.29302888197623</v>
       </c>
-      <c r="AN7">
+      <c r="AN5">
         <f t="shared" si="2"/>
         <v>643.63435457769162</v>
       </c>
-      <c r="AO7">
+      <c r="AO5">
         <f t="shared" si="2"/>
         <v>11.182546796826877</v>
       </c>
-      <c r="AP7">
+      <c r="AP5">
         <f t="shared" si="2"/>
         <v>451.20800831854399</v>
       </c>
-      <c r="AQ7">
+      <c r="AQ5">
         <f t="shared" si="2"/>
         <v>-11.227312397529944</v>
       </c>
-      <c r="AR7">
+      <c r="AR5">
         <f t="shared" si="2"/>
         <v>0.16242426207365368</v>
       </c>
-      <c r="AS7">
+      <c r="AS5">
         <f t="shared" si="2"/>
         <v>0.61451440865077123</v>
       </c>
-      <c r="AT7">
+      <c r="AT5">
         <f t="shared" si="2"/>
         <v>0.26500379404034702</v>
       </c>
-      <c r="AU7">
+      <c r="AU5">
         <f t="shared" si="2"/>
         <v>0.18062961903233468</v>
       </c>
-      <c r="AV7">
+      <c r="AV5">
         <f t="shared" si="2"/>
         <v>0.75597625347011377</v>
       </c>
-      <c r="AW7">
+      <c r="AW5">
         <f t="shared" si="2"/>
         <v>0.11037680297071474</v>
       </c>
-      <c r="AX7">
+      <c r="AX5">
         <f t="shared" si="2"/>
         <v>0.14104335342573704</v>
       </c>
-      <c r="AY7">
+      <c r="AY5">
         <f t="shared" si="2"/>
         <v>1.0389143498748852</v>
       </c>
-      <c r="AZ7">
+      <c r="AZ5">
         <f t="shared" si="2"/>
         <v>-0.23588096141925249</v>
       </c>
-      <c r="BA7">
+      <c r="BA5">
         <f t="shared" si="2"/>
         <v>0.14090008419083738</v>
       </c>
-      <c r="BB7">
+      <c r="BB5">
         <f t="shared" si="2"/>
         <v>0.70063962460794293</v>
       </c>
-      <c r="BC7">
+      <c r="BC5">
         <f t="shared" si="2"/>
         <v>8.9188190652010585E-2</v>
       </c>
-      <c r="BD7">
+      <c r="BD5">
         <f t="shared" si="2"/>
         <v>0.11777381843009882</v>
       </c>
-      <c r="BE7">
+      <c r="BE5">
         <f t="shared" si="2"/>
         <v>0.44317221398122963</v>
       </c>
-      <c r="BF7">
+      <c r="BF5">
         <f t="shared" si="2"/>
         <v>-9.0366222389410999E-2</v>
       </c>
-      <c r="BG7">
+      <c r="BG5">
         <f t="shared" si="2"/>
         <v>-6.3410999470138119E-2</v>
       </c>
-      <c r="BH7">
+      <c r="BH5">
         <f t="shared" si="2"/>
         <v>0.10397305703802344</v>
       </c>
-      <c r="BI7">
+      <c r="BI5">
         <f t="shared" si="2"/>
         <v>-0.13945304367484335</v>
       </c>
-      <c r="BJ7">
+      <c r="BJ5">
         <f t="shared" si="2"/>
         <v>0.11930271005663372</v>
       </c>
-      <c r="BK7">
+      <c r="BK5">
         <f t="shared" si="2"/>
         <v>6.2453890727801914E-2</v>
       </c>
-      <c r="BL7">
+      <c r="BL5">
         <f t="shared" si="2"/>
         <v>-5.0150728612866485E-3</v>
       </c>
-      <c r="BM7">
+      <c r="BM5">
         <f t="shared" si="2"/>
         <v>0.14409355445069613</v>
       </c>
-      <c r="BN7">
+      <c r="BN5">
         <f t="shared" si="2"/>
         <v>1.6517832046057734E-2</v>
       </c>
-      <c r="BO7">
+      <c r="BO5">
         <f t="shared" si="2"/>
         <v>77.28267217046853</v>
       </c>
-      <c r="BP7">
-        <f t="shared" ref="BP7" si="3">BP3-BP4</f>
+      <c r="BP5">
+        <f t="shared" ref="BP5" si="3">BP2-BP3</f>
         <v>74.259740045628462</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>72</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B8" t="s">
         <v>73</v>
       </c>
     </row>

</xml_diff>